<commit_message>
Update Sectoral emissions 2021 scenario file
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_SectoralEmissions_2021.xlsx
+++ b/SuppXLS/Scen_SectoralEmissions_2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TIM-2.0\TIMES-Ireland-model-CB\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E946E095-5592-42EE-991C-8F7CE762B65E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8005B761-7EB9-4F5D-AB42-AD11F311B2D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="24" r:id="rId1"/>
@@ -160,7 +160,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="123">
   <si>
     <t>LimType</t>
   </si>
@@ -546,6 +546,9 @@
   </si>
   <si>
     <t>NET</t>
+  </si>
+  <si>
+    <t>FX</t>
   </si>
 </sst>
 </file>
@@ -1635,8 +1638,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:Z99"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView showGridLines="0" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5511,8 +5514,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7:G11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7:H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5627,7 +5630,7 @@
         <v>121</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>68</v>
+        <v>122</v>
       </c>
       <c r="I7" s="8">
         <v>1</v>
@@ -5657,7 +5660,7 @@
         <v>121</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>68</v>
+        <v>122</v>
       </c>
       <c r="I8" s="8">
         <v>1</v>
@@ -5687,7 +5690,7 @@
         <v>121</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>68</v>
+        <v>122</v>
       </c>
       <c r="I9" s="8">
         <v>1</v>
@@ -5717,7 +5720,7 @@
         <v>121</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>68</v>
+        <v>122</v>
       </c>
       <c r="I10" s="8">
         <v>1</v>
@@ -5747,7 +5750,7 @@
         <v>121</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>68</v>
+        <v>122</v>
       </c>
       <c r="I11" s="8">
         <v>1</v>
@@ -5788,8 +5791,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7:G11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Update scenario file-Sectoral carbon budgets 2021
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_SectoralEmissions_2021.xlsx
+++ b/SuppXLS/Scen_SectoralEmissions_2021.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TIM-2.0\TIMES-Ireland-model-CB\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agaur\Documents\Veda\times-ireland-model-sectoral_cb\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8005B761-7EB9-4F5D-AB42-AD11F311B2D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C21B850-4AC6-47D7-B69F-B0F36C32DAD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="12600" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="24" r:id="rId1"/>
@@ -160,7 +160,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="121">
   <si>
     <t>LimType</t>
   </si>
@@ -386,9 +386,6 @@
     <t>UC_RHS</t>
   </si>
   <si>
-    <t>UP</t>
-  </si>
-  <si>
     <t>*Units</t>
   </si>
   <si>
@@ -404,9 +401,6 @@
     <t>~UC_Sets: T_S:</t>
   </si>
   <si>
-    <t>UC_CUMCOM</t>
-  </si>
-  <si>
     <t>Other_indexes</t>
   </si>
   <si>
@@ -416,9 +410,6 @@
     <t>*CO2*,-*CO2S</t>
   </si>
   <si>
-    <t>UC_CUMFLO</t>
-  </si>
-  <si>
     <t>Pset_PN</t>
   </si>
   <si>
@@ -545,7 +536,10 @@
     <t>CO2 emissions 2021 in Agri- multi</t>
   </si>
   <si>
-    <t>NET</t>
+    <t>UC_COMNET</t>
+  </si>
+  <si>
+    <t>UC_FLO</t>
   </si>
   <si>
     <t>FX</t>
@@ -1642,21 +1636,21 @@
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="21.7265625" style="8" customWidth="1"/>
-    <col min="5" max="6" width="14.1796875" style="8" customWidth="1"/>
-    <col min="7" max="7" width="12.1796875" style="8" customWidth="1"/>
-    <col min="8" max="10" width="8.1796875" style="8" customWidth="1"/>
-    <col min="11" max="11" width="9.7265625" style="8" customWidth="1"/>
-    <col min="12" max="12" width="8.1796875" style="8" customWidth="1"/>
+    <col min="1" max="4" width="21.7109375" style="8" customWidth="1"/>
+    <col min="5" max="6" width="14.140625" style="8" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" style="8" customWidth="1"/>
+    <col min="8" max="10" width="8.140625" style="8" customWidth="1"/>
+    <col min="11" max="11" width="9.7109375" style="8" customWidth="1"/>
+    <col min="12" max="12" width="8.140625" style="8" customWidth="1"/>
     <col min="13" max="13" width="10" style="8" customWidth="1"/>
-    <col min="14" max="14" width="11.453125" style="8" customWidth="1"/>
-    <col min="15" max="15" width="13.453125" style="8" customWidth="1"/>
-    <col min="16" max="16384" width="8.81640625" style="8"/>
+    <col min="14" max="14" width="11.42578125" style="8" customWidth="1"/>
+    <col min="15" max="15" width="13.42578125" style="8" customWidth="1"/>
+    <col min="16" max="16384" width="8.85546875" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="16"/>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -1684,7 +1678,7 @@
       <c r="Y1" s="17"/>
       <c r="Z1" s="17"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="16"/>
       <c r="B2" s="16"/>
       <c r="C2" s="16"/>
@@ -1712,7 +1706,7 @@
       <c r="Y2" s="17"/>
       <c r="Z2" s="17"/>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="16"/>
       <c r="B3" s="16"/>
       <c r="C3" s="16"/>
@@ -1740,7 +1734,7 @@
       <c r="Y3" s="17"/>
       <c r="Z3" s="17"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="16"/>
       <c r="B4" s="16"/>
       <c r="C4" s="16"/>
@@ -1768,7 +1762,7 @@
       <c r="Y4" s="17"/>
       <c r="Z4" s="17"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
       <c r="B5" s="16"/>
       <c r="C5" s="16"/>
@@ -1796,7 +1790,7 @@
       <c r="Y5" s="17"/>
       <c r="Z5" s="17"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="16"/>
       <c r="B6" s="16"/>
       <c r="C6" s="16"/>
@@ -1824,7 +1818,7 @@
       <c r="Y6" s="17"/>
       <c r="Z6" s="17"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="16"/>
       <c r="B7" s="16"/>
       <c r="C7" s="16"/>
@@ -1852,7 +1846,7 @@
       <c r="Y7" s="17"/>
       <c r="Z7" s="17"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="16"/>
       <c r="B8" s="16"/>
       <c r="C8" s="16"/>
@@ -1880,7 +1874,7 @@
       <c r="Y8" s="17"/>
       <c r="Z8" s="17"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="16"/>
       <c r="B9" s="16"/>
       <c r="C9" s="16"/>
@@ -1908,7 +1902,7 @@
       <c r="Y9" s="17"/>
       <c r="Z9" s="17"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="16"/>
       <c r="B10" s="16"/>
       <c r="C10" s="16"/>
@@ -1936,7 +1930,7 @@
       <c r="Y10" s="17"/>
       <c r="Z10" s="17"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="16"/>
       <c r="B11" s="16"/>
       <c r="C11" s="16"/>
@@ -1964,7 +1958,7 @@
       <c r="Y11" s="17"/>
       <c r="Z11" s="17"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="16"/>
       <c r="B12" s="16"/>
       <c r="C12" s="16"/>
@@ -1992,7 +1986,7 @@
       <c r="Y12" s="17"/>
       <c r="Z12" s="17"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="16"/>
       <c r="B13" s="16"/>
       <c r="C13" s="16"/>
@@ -2020,7 +2014,7 @@
       <c r="Y13" s="17"/>
       <c r="Z13" s="17"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="16"/>
       <c r="B14" s="16"/>
       <c r="C14" s="16"/>
@@ -2048,7 +2042,7 @@
       <c r="Y14" s="17"/>
       <c r="Z14" s="17"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="16"/>
       <c r="B15" s="16"/>
       <c r="C15" s="16"/>
@@ -2076,9 +2070,9 @@
       <c r="Y15" s="17"/>
       <c r="Z15" s="17"/>
     </row>
-    <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="33" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B16" s="33"/>
       <c r="C16" s="33"/>
@@ -2106,7 +2100,7 @@
       <c r="Y16" s="17"/>
       <c r="Z16" s="17"/>
     </row>
-    <row r="17" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="20"/>
       <c r="B17" s="20"/>
       <c r="C17" s="20"/>
@@ -2134,7 +2128,7 @@
       <c r="Y17" s="17"/>
       <c r="Z17" s="17"/>
     </row>
-    <row r="18" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="20"/>
       <c r="B18" s="20"/>
       <c r="C18" s="20"/>
@@ -2162,12 +2156,12 @@
       <c r="Y18" s="17"/>
       <c r="Z18" s="17"/>
     </row>
-    <row r="19" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="23" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B19" s="32" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C19" s="32"/>
       <c r="D19" s="32"/>
@@ -2194,12 +2188,12 @@
       <c r="Y19" s="17"/>
       <c r="Z19" s="17"/>
     </row>
-    <row r="20" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="23" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B20" s="32" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C20" s="32"/>
       <c r="D20" s="32"/>
@@ -2226,12 +2220,12 @@
       <c r="Y20" s="17"/>
       <c r="Z20" s="17"/>
     </row>
-    <row r="21" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="23" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B21" s="26" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C21" s="26"/>
       <c r="D21" s="26"/>
@@ -2258,7 +2252,7 @@
       <c r="Y21" s="17"/>
       <c r="Z21" s="17"/>
     </row>
-    <row r="22" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="23"/>
       <c r="B22" s="26"/>
       <c r="C22" s="26"/>
@@ -2286,12 +2280,12 @@
       <c r="Y22" s="17"/>
       <c r="Z22" s="17"/>
     </row>
-    <row r="23" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="23" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B23" s="32" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C23" s="32"/>
       <c r="D23" s="32"/>
@@ -2318,10 +2312,10 @@
       <c r="Y23" s="17"/>
       <c r="Z23" s="17"/>
     </row>
-    <row r="24" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="23"/>
       <c r="B24" s="26" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C24" s="26"/>
       <c r="D24" s="26"/>
@@ -2348,7 +2342,7 @@
       <c r="Y24" s="17"/>
       <c r="Z24" s="17"/>
     </row>
-    <row r="25" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="23"/>
       <c r="B25" s="26"/>
       <c r="C25" s="26"/>
@@ -2376,12 +2370,12 @@
       <c r="Y25" s="17"/>
       <c r="Z25" s="17"/>
     </row>
-    <row r="26" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="23" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B26" s="32" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C26" s="32"/>
       <c r="D26" s="32"/>
@@ -2408,7 +2402,7 @@
       <c r="Y26" s="17"/>
       <c r="Z26" s="17"/>
     </row>
-    <row r="27" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="23"/>
       <c r="B27" s="26"/>
       <c r="C27" s="26"/>
@@ -2436,7 +2430,7 @@
       <c r="Y27" s="17"/>
       <c r="Z27" s="17"/>
     </row>
-    <row r="28" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="23"/>
       <c r="B28" s="26"/>
       <c r="C28" s="26"/>
@@ -2464,9 +2458,9 @@
       <c r="Y28" s="17"/>
       <c r="Z28" s="17"/>
     </row>
-    <row r="29" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="23" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B29" s="27">
         <v>1</v>
@@ -2496,12 +2490,12 @@
       <c r="Y29" s="17"/>
       <c r="Z29" s="17"/>
     </row>
-    <row r="30" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="23" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B30" s="34" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C30" s="32"/>
       <c r="D30" s="32"/>
@@ -2528,12 +2522,12 @@
       <c r="Y30" s="17"/>
       <c r="Z30" s="17"/>
     </row>
-    <row r="31" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="23" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B31" s="32" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C31" s="32"/>
       <c r="D31" s="32"/>
@@ -2560,10 +2554,10 @@
       <c r="Y31" s="17"/>
       <c r="Z31" s="17"/>
     </row>
-    <row r="32" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="29"/>
       <c r="B32" s="30" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C32" s="29"/>
       <c r="D32" s="29"/>
@@ -2590,7 +2584,7 @@
       <c r="Y32" s="17"/>
       <c r="Z32" s="17"/>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A33" s="16"/>
       <c r="B33" s="16"/>
       <c r="C33" s="16"/>
@@ -2618,7 +2612,7 @@
       <c r="Y33" s="17"/>
       <c r="Z33" s="17"/>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A34" s="16"/>
       <c r="B34" s="16"/>
       <c r="C34" s="16"/>
@@ -2646,7 +2640,7 @@
       <c r="Y34" s="17"/>
       <c r="Z34" s="17"/>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A35" s="16"/>
       <c r="B35" s="16"/>
       <c r="C35" s="16"/>
@@ -2674,7 +2668,7 @@
       <c r="Y35" s="17"/>
       <c r="Z35" s="17"/>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A36" s="16"/>
       <c r="B36" s="16"/>
       <c r="C36" s="16"/>
@@ -2702,7 +2696,7 @@
       <c r="Y36" s="17"/>
       <c r="Z36" s="17"/>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A37" s="16"/>
       <c r="B37" s="16"/>
       <c r="C37" s="16"/>
@@ -2730,7 +2724,7 @@
       <c r="Y37" s="17"/>
       <c r="Z37" s="17"/>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A38" s="16"/>
       <c r="B38" s="16"/>
       <c r="C38" s="16"/>
@@ -2758,7 +2752,7 @@
       <c r="Y38" s="17"/>
       <c r="Z38" s="17"/>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A39" s="16"/>
       <c r="B39" s="16"/>
       <c r="C39" s="16"/>
@@ -2786,7 +2780,7 @@
       <c r="Y39" s="17"/>
       <c r="Z39" s="17"/>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A40" s="16"/>
       <c r="B40" s="16"/>
       <c r="C40" s="16"/>
@@ -2814,7 +2808,7 @@
       <c r="Y40" s="17"/>
       <c r="Z40" s="17"/>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A41" s="16"/>
       <c r="B41" s="16"/>
       <c r="C41" s="16"/>
@@ -2842,7 +2836,7 @@
       <c r="Y41" s="17"/>
       <c r="Z41" s="17"/>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A42" s="16"/>
       <c r="B42" s="16"/>
       <c r="C42" s="16"/>
@@ -2870,7 +2864,7 @@
       <c r="Y42" s="17"/>
       <c r="Z42" s="17"/>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A43" s="17"/>
       <c r="B43" s="17"/>
       <c r="C43" s="17"/>
@@ -2898,7 +2892,7 @@
       <c r="Y43" s="17"/>
       <c r="Z43" s="17"/>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A44" s="17"/>
       <c r="B44" s="17"/>
       <c r="C44" s="17"/>
@@ -2926,7 +2920,7 @@
       <c r="Y44" s="17"/>
       <c r="Z44" s="17"/>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A45" s="17"/>
       <c r="B45" s="17"/>
       <c r="C45" s="17"/>
@@ -2954,7 +2948,7 @@
       <c r="Y45" s="17"/>
       <c r="Z45" s="17"/>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A46" s="17"/>
       <c r="B46" s="17"/>
       <c r="C46" s="17"/>
@@ -2982,7 +2976,7 @@
       <c r="Y46" s="17"/>
       <c r="Z46" s="17"/>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A47" s="17"/>
       <c r="B47" s="17"/>
       <c r="C47" s="17"/>
@@ -3010,7 +3004,7 @@
       <c r="Y47" s="17"/>
       <c r="Z47" s="17"/>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A48" s="17"/>
       <c r="B48" s="17"/>
       <c r="C48" s="17"/>
@@ -3038,7 +3032,7 @@
       <c r="Y48" s="17"/>
       <c r="Z48" s="17"/>
     </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A49" s="17"/>
       <c r="B49" s="17"/>
       <c r="C49" s="17"/>
@@ -3066,7 +3060,7 @@
       <c r="Y49" s="17"/>
       <c r="Z49" s="17"/>
     </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A50" s="17"/>
       <c r="B50" s="17"/>
       <c r="C50" s="17"/>
@@ -3094,7 +3088,7 @@
       <c r="Y50" s="17"/>
       <c r="Z50" s="17"/>
     </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A51" s="17"/>
       <c r="B51" s="17"/>
       <c r="C51" s="17"/>
@@ -3122,7 +3116,7 @@
       <c r="Y51" s="17"/>
       <c r="Z51" s="17"/>
     </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A52" s="17"/>
       <c r="B52" s="17"/>
       <c r="C52" s="17"/>
@@ -3150,7 +3144,7 @@
       <c r="Y52" s="17"/>
       <c r="Z52" s="17"/>
     </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A53" s="17"/>
       <c r="B53" s="17"/>
       <c r="C53" s="17"/>
@@ -3178,7 +3172,7 @@
       <c r="Y53" s="17"/>
       <c r="Z53" s="17"/>
     </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A54" s="17"/>
       <c r="B54" s="17"/>
       <c r="C54" s="17"/>
@@ -3206,7 +3200,7 @@
       <c r="Y54" s="17"/>
       <c r="Z54" s="17"/>
     </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A55" s="17"/>
       <c r="B55" s="17"/>
       <c r="C55" s="17"/>
@@ -3234,7 +3228,7 @@
       <c r="Y55" s="17"/>
       <c r="Z55" s="17"/>
     </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A56" s="17"/>
       <c r="B56" s="17"/>
       <c r="C56" s="17"/>
@@ -3262,7 +3256,7 @@
       <c r="Y56" s="17"/>
       <c r="Z56" s="17"/>
     </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A57" s="17"/>
       <c r="B57" s="17"/>
       <c r="C57" s="17"/>
@@ -3290,7 +3284,7 @@
       <c r="Y57" s="17"/>
       <c r="Z57" s="17"/>
     </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A58" s="17"/>
       <c r="B58" s="17"/>
       <c r="C58" s="17"/>
@@ -3318,7 +3312,7 @@
       <c r="Y58" s="17"/>
       <c r="Z58" s="17"/>
     </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A59" s="17"/>
       <c r="B59" s="17"/>
       <c r="C59" s="17"/>
@@ -3346,7 +3340,7 @@
       <c r="Y59" s="17"/>
       <c r="Z59" s="17"/>
     </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A60" s="17"/>
       <c r="B60" s="17"/>
       <c r="C60" s="17"/>
@@ -3374,7 +3368,7 @@
       <c r="Y60" s="17"/>
       <c r="Z60" s="17"/>
     </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A61" s="17"/>
       <c r="B61" s="17"/>
       <c r="C61" s="17"/>
@@ -3402,7 +3396,7 @@
       <c r="Y61" s="17"/>
       <c r="Z61" s="17"/>
     </row>
-    <row r="62" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A62" s="17"/>
       <c r="B62" s="17"/>
       <c r="C62" s="17"/>
@@ -3430,7 +3424,7 @@
       <c r="Y62" s="17"/>
       <c r="Z62" s="17"/>
     </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A63" s="17"/>
       <c r="B63" s="17"/>
       <c r="C63" s="17"/>
@@ -3458,7 +3452,7 @@
       <c r="Y63" s="17"/>
       <c r="Z63" s="17"/>
     </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A64" s="17"/>
       <c r="B64" s="17"/>
       <c r="C64" s="17"/>
@@ -3486,7 +3480,7 @@
       <c r="Y64" s="17"/>
       <c r="Z64" s="17"/>
     </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A65" s="17"/>
       <c r="B65" s="17"/>
       <c r="C65" s="17"/>
@@ -3514,7 +3508,7 @@
       <c r="Y65" s="17"/>
       <c r="Z65" s="17"/>
     </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A66" s="17"/>
       <c r="B66" s="17"/>
       <c r="C66" s="17"/>
@@ -3542,7 +3536,7 @@
       <c r="Y66" s="17"/>
       <c r="Z66" s="17"/>
     </row>
-    <row r="67" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A67" s="17"/>
       <c r="B67" s="17"/>
       <c r="C67" s="17"/>
@@ -3570,7 +3564,7 @@
       <c r="Y67" s="17"/>
       <c r="Z67" s="17"/>
     </row>
-    <row r="68" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A68" s="17"/>
       <c r="B68" s="17"/>
       <c r="C68" s="17"/>
@@ -3598,7 +3592,7 @@
       <c r="Y68" s="17"/>
       <c r="Z68" s="17"/>
     </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A69" s="17"/>
       <c r="B69" s="17"/>
       <c r="C69" s="17"/>
@@ -3626,7 +3620,7 @@
       <c r="Y69" s="17"/>
       <c r="Z69" s="17"/>
     </row>
-    <row r="70" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A70" s="17"/>
       <c r="B70" s="17"/>
       <c r="C70" s="17"/>
@@ -3654,7 +3648,7 @@
       <c r="Y70" s="17"/>
       <c r="Z70" s="17"/>
     </row>
-    <row r="71" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A71" s="17"/>
       <c r="B71" s="17"/>
       <c r="C71" s="17"/>
@@ -3682,7 +3676,7 @@
       <c r="Y71" s="17"/>
       <c r="Z71" s="17"/>
     </row>
-    <row r="72" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A72" s="17"/>
       <c r="B72" s="17"/>
       <c r="C72" s="17"/>
@@ -3710,7 +3704,7 @@
       <c r="Y72" s="17"/>
       <c r="Z72" s="17"/>
     </row>
-    <row r="73" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A73" s="17"/>
       <c r="B73" s="17"/>
       <c r="C73" s="17"/>
@@ -3738,7 +3732,7 @@
       <c r="Y73" s="17"/>
       <c r="Z73" s="17"/>
     </row>
-    <row r="74" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A74" s="17"/>
       <c r="B74" s="17"/>
       <c r="C74" s="17"/>
@@ -3766,7 +3760,7 @@
       <c r="Y74" s="17"/>
       <c r="Z74" s="17"/>
     </row>
-    <row r="75" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A75" s="17"/>
       <c r="B75" s="17"/>
       <c r="C75" s="17"/>
@@ -3794,7 +3788,7 @@
       <c r="Y75" s="17"/>
       <c r="Z75" s="17"/>
     </row>
-    <row r="76" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A76" s="17"/>
       <c r="B76" s="17"/>
       <c r="C76" s="17"/>
@@ -3822,7 +3816,7 @@
       <c r="Y76" s="17"/>
       <c r="Z76" s="17"/>
     </row>
-    <row r="77" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A77" s="17"/>
       <c r="B77" s="17"/>
       <c r="C77" s="17"/>
@@ -3850,7 +3844,7 @@
       <c r="Y77" s="17"/>
       <c r="Z77" s="17"/>
     </row>
-    <row r="78" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A78" s="17"/>
       <c r="B78" s="17"/>
       <c r="C78" s="17"/>
@@ -3878,7 +3872,7 @@
       <c r="Y78" s="17"/>
       <c r="Z78" s="17"/>
     </row>
-    <row r="79" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A79" s="17"/>
       <c r="B79" s="17"/>
       <c r="C79" s="17"/>
@@ -3906,7 +3900,7 @@
       <c r="Y79" s="17"/>
       <c r="Z79" s="17"/>
     </row>
-    <row r="80" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A80" s="17"/>
       <c r="B80" s="17"/>
       <c r="C80" s="17"/>
@@ -3934,7 +3928,7 @@
       <c r="Y80" s="17"/>
       <c r="Z80" s="17"/>
     </row>
-    <row r="81" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A81" s="17"/>
       <c r="B81" s="17"/>
       <c r="C81" s="17"/>
@@ -3962,7 +3956,7 @@
       <c r="Y81" s="17"/>
       <c r="Z81" s="17"/>
     </row>
-    <row r="82" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A82" s="17"/>
       <c r="B82" s="17"/>
       <c r="C82" s="17"/>
@@ -3990,7 +3984,7 @@
       <c r="Y82" s="17"/>
       <c r="Z82" s="17"/>
     </row>
-    <row r="83" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A83" s="17"/>
       <c r="B83" s="17"/>
       <c r="C83" s="17"/>
@@ -4018,7 +4012,7 @@
       <c r="Y83" s="17"/>
       <c r="Z83" s="17"/>
     </row>
-    <row r="84" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A84" s="17"/>
       <c r="B84" s="17"/>
       <c r="C84" s="17"/>
@@ -4046,7 +4040,7 @@
       <c r="Y84" s="17"/>
       <c r="Z84" s="17"/>
     </row>
-    <row r="85" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A85" s="17"/>
       <c r="B85" s="17"/>
       <c r="C85" s="17"/>
@@ -4074,7 +4068,7 @@
       <c r="Y85" s="17"/>
       <c r="Z85" s="17"/>
     </row>
-    <row r="86" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A86" s="17"/>
       <c r="B86" s="17"/>
       <c r="C86" s="17"/>
@@ -4102,7 +4096,7 @@
       <c r="Y86" s="17"/>
       <c r="Z86" s="17"/>
     </row>
-    <row r="87" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A87" s="17"/>
       <c r="B87" s="17"/>
       <c r="C87" s="17"/>
@@ -4130,7 +4124,7 @@
       <c r="Y87" s="17"/>
       <c r="Z87" s="17"/>
     </row>
-    <row r="88" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A88" s="17"/>
       <c r="B88" s="17"/>
       <c r="C88" s="17"/>
@@ -4158,7 +4152,7 @@
       <c r="Y88" s="17"/>
       <c r="Z88" s="17"/>
     </row>
-    <row r="89" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A89" s="17"/>
       <c r="B89" s="17"/>
       <c r="C89" s="17"/>
@@ -4186,7 +4180,7 @@
       <c r="Y89" s="17"/>
       <c r="Z89" s="17"/>
     </row>
-    <row r="90" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A90" s="17"/>
       <c r="B90" s="17"/>
       <c r="C90" s="17"/>
@@ -4214,7 +4208,7 @@
       <c r="Y90" s="17"/>
       <c r="Z90" s="17"/>
     </row>
-    <row r="91" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A91" s="17"/>
       <c r="B91" s="17"/>
       <c r="C91" s="17"/>
@@ -4242,7 +4236,7 @@
       <c r="Y91" s="17"/>
       <c r="Z91" s="17"/>
     </row>
-    <row r="92" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A92" s="17"/>
       <c r="B92" s="17"/>
       <c r="C92" s="17"/>
@@ -4270,7 +4264,7 @@
       <c r="Y92" s="17"/>
       <c r="Z92" s="17"/>
     </row>
-    <row r="93" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A93" s="17"/>
       <c r="B93" s="17"/>
       <c r="C93" s="17"/>
@@ -4298,7 +4292,7 @@
       <c r="Y93" s="17"/>
       <c r="Z93" s="17"/>
     </row>
-    <row r="94" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A94" s="17"/>
       <c r="B94" s="17"/>
       <c r="C94" s="17"/>
@@ -4326,7 +4320,7 @@
       <c r="Y94" s="17"/>
       <c r="Z94" s="17"/>
     </row>
-    <row r="95" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A95" s="17"/>
       <c r="B95" s="17"/>
       <c r="C95" s="17"/>
@@ -4354,7 +4348,7 @@
       <c r="Y95" s="17"/>
       <c r="Z95" s="17"/>
     </row>
-    <row r="96" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A96" s="17"/>
       <c r="B96" s="17"/>
       <c r="C96" s="17"/>
@@ -4382,7 +4376,7 @@
       <c r="Y96" s="17"/>
       <c r="Z96" s="17"/>
     </row>
-    <row r="97" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A97" s="17"/>
       <c r="B97" s="17"/>
       <c r="C97" s="17"/>
@@ -4410,7 +4404,7 @@
       <c r="Y97" s="17"/>
       <c r="Z97" s="17"/>
     </row>
-    <row r="98" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A98" s="17"/>
       <c r="B98" s="17"/>
       <c r="C98" s="17"/>
@@ -4438,7 +4432,7 @@
       <c r="Y98" s="17"/>
       <c r="Z98" s="17"/>
     </row>
-    <row r="99" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A99" s="17"/>
       <c r="B99" s="17"/>
       <c r="C99" s="17"/>
@@ -4495,40 +4489,40 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.1796875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7265625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="3.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="5.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="6.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="4.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7.54296875" style="1" customWidth="1"/>
-    <col min="25" max="25" width="6.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="6.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="3.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.5703125" style="1" customWidth="1"/>
+    <col min="25" max="25" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="27" max="28" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="5.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="6.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="16384" width="9.1796875" style="1"/>
+    <col min="29" max="29" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="C3" s="2" t="str" cm="1">
         <f t="array" ref="C3">IF(LEFT(INDEX(C5:C7,$A$4),1)&lt;&gt;"*",INDEX(C5:C7,$A$4),"")</f>
         <v>IE</v>
@@ -4642,12 +4636,12 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>27</v>
       </c>
@@ -4762,7 +4756,7 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>30</v>
       </c>
@@ -4879,7 +4873,7 @@
         <v>*IE-MN</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>31</v>
       </c>
@@ -4996,7 +4990,7 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="10" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>32</v>
       </c>
@@ -5004,7 +4998,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>34</v>
       </c>
@@ -5012,7 +5006,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>35</v>
       </c>
@@ -5020,7 +5014,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>36</v>
       </c>
@@ -5028,7 +5022,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>37</v>
       </c>
@@ -5036,7 +5030,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>38</v>
       </c>
@@ -5044,7 +5038,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>39</v>
       </c>
@@ -5052,7 +5046,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>40</v>
       </c>
@@ -5060,7 +5054,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>41</v>
       </c>
@@ -5068,7 +5062,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>42</v>
       </c>
@@ -5076,7 +5070,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>43</v>
       </c>
@@ -5084,7 +5078,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>44</v>
       </c>
@@ -5092,7 +5086,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>45</v>
       </c>
@@ -5100,7 +5094,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>46</v>
       </c>
@@ -5108,7 +5102,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>47</v>
       </c>
@@ -5116,7 +5110,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>48</v>
       </c>
@@ -5124,7 +5118,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>49</v>
       </c>
@@ -5132,7 +5126,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>50</v>
       </c>
@@ -5140,7 +5134,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>51</v>
       </c>
@@ -5148,7 +5142,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>52</v>
       </c>
@@ -5156,7 +5150,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>53</v>
       </c>
@@ -5164,7 +5158,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>54</v>
       </c>
@@ -5172,7 +5166,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>55</v>
       </c>
@@ -5180,7 +5174,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>56</v>
       </c>
@@ -5188,7 +5182,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>57</v>
       </c>
@@ -5196,7 +5190,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
         <v>58</v>
       </c>
@@ -5204,7 +5198,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
         <v>59</v>
       </c>
@@ -5212,7 +5206,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
         <v>60</v>
       </c>
@@ -5262,64 +5256,64 @@
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" style="8"/>
+    <col min="1" max="1" width="9.140625" style="8"/>
     <col min="2" max="2" width="14" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.1796875" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.140625" style="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="12" width="9.1796875" style="8"/>
-    <col min="13" max="13" width="10.54296875" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="12" width="9.140625" style="8"/>
+    <col min="13" max="13" width="10.5703125" style="8" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12" style="8" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.1796875" style="8"/>
+    <col min="15" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C1" s="31" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D1" s="31" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C2" s="8" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D2" s="8">
         <f>[1]Sheet1!$D$156</f>
         <v>10.173999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C3" s="8" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D3" s="35">
         <f>[1]Sheet1!$D$157</f>
         <v>8.68032</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C4" s="8" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D4" s="35"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C5" s="8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D5" s="8">
         <f>[1]Sheet1!$D$155</f>
         <v>10.087999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6"/>
       <c r="B6"/>
       <c r="C6" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D6" s="35">
         <f>[1]Sheet1!$D$158</f>
@@ -5339,11 +5333,11 @@
       <c r="P6"/>
       <c r="Q6"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7"/>
       <c r="B7"/>
       <c r="C7" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D7" s="35"/>
       <c r="E7"/>
@@ -5360,16 +5354,16 @@
       <c r="P7"/>
       <c r="Q7"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C8" s="8" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D8" s="8">
         <f>[1]Sheet1!$D$159</f>
         <v>22.391718679361578</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10"/>
       <c r="B10"/>
       <c r="C10"/>
@@ -5388,7 +5382,7 @@
       <c r="P10"/>
       <c r="Q10"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11"/>
       <c r="B11"/>
       <c r="E11"/>
@@ -5405,7 +5399,7 @@
       <c r="P11"/>
       <c r="Q11"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12"/>
       <c r="B12"/>
       <c r="C12"/>
@@ -5423,7 +5417,7 @@
       <c r="P12"/>
       <c r="Q12"/>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21"/>
       <c r="B21"/>
       <c r="C21"/>
@@ -5441,7 +5435,7 @@
       <c r="P21"/>
       <c r="Q21"/>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22"/>
       <c r="B22"/>
       <c r="C22"/>
@@ -5460,7 +5454,7 @@
       <c r="P22"/>
       <c r="Q22"/>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23"/>
       <c r="B23"/>
       <c r="C23"/>
@@ -5479,7 +5473,7 @@
       <c r="P23"/>
       <c r="Q23"/>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24"/>
       <c r="B24"/>
       <c r="C24"/>
@@ -5514,50 +5508,50 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7:H11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" style="8"/>
+    <col min="1" max="1" width="9.140625" style="8"/>
     <col min="2" max="2" width="31" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.54296875" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.1796875" style="8"/>
-    <col min="5" max="5" width="16.453125" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.26953125" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.1796875" style="8"/>
-    <col min="9" max="9" width="13.1796875" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.1796875" style="8" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="8"/>
+    <col min="5" max="5" width="16.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="8"/>
+    <col min="9" max="9" width="13.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" style="8" customWidth="1"/>
     <col min="11" max="11" width="12" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="27.81640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.1796875" style="8"/>
+    <col min="12" max="12" width="27.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="str">
         <f>"~UC_Sets: R_E: "  &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!C3)</f>
         <v>~UC_Sets: R_E: IE</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B3" s="11" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H4" s="8" t="str">
         <f>IF(RIGHT(B2,1)&lt;&gt;" ","~UC_T","")</f>
         <v>~UC_T</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B5" s="12" t="s">
         <v>61</v>
       </c>
@@ -5565,25 +5559,25 @@
         <v>62</v>
       </c>
       <c r="D5" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="F5" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="E5" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="F5" s="13" t="s">
-        <v>72</v>
-      </c>
       <c r="G5" s="13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H5" s="13" t="s">
         <v>0</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>74</v>
+        <v>118</v>
       </c>
       <c r="J5" s="14" t="s">
-        <v>78</v>
+        <v>119</v>
       </c>
       <c r="K5" s="10" t="s">
         <v>65</v>
@@ -5592,9 +5586,9 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B6" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
@@ -5605,19 +5599,19 @@
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
       <c r="K6" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L6" s="15"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E7" s="8" t="str">
         <f>config!C2</f>
@@ -5626,11 +5620,8 @@
       <c r="F7" s="8">
         <v>2021</v>
       </c>
-      <c r="G7" s="8" t="s">
-        <v>121</v>
-      </c>
       <c r="H7" s="8" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="I7" s="8">
         <v>1</v>
@@ -5640,27 +5631,24 @@
         <v>10174</v>
       </c>
       <c r="L7" s="8" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C8" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="F8" s="8">
         <v>2021</v>
       </c>
-      <c r="G8" s="8" t="s">
-        <v>121</v>
-      </c>
       <c r="H8" s="8" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="I8" s="8">
         <v>1</v>
@@ -5670,27 +5658,24 @@
         <v>8680.32</v>
       </c>
       <c r="L8" s="8" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C9" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F9" s="8">
         <v>2021</v>
       </c>
-      <c r="G9" s="8" t="s">
-        <v>121</v>
-      </c>
       <c r="H9" s="8" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="I9" s="8">
         <v>1</v>
@@ -5700,27 +5685,24 @@
         <v>10088</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C10" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F10" s="8">
         <v>2021</v>
       </c>
-      <c r="G10" s="8" t="s">
-        <v>121</v>
-      </c>
       <c r="H10" s="8" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="I10" s="8">
         <v>1</v>
@@ -5730,27 +5712,24 @@
         <v>9817.9359360518702</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C11" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F11" s="8">
         <v>2021</v>
       </c>
-      <c r="G11" s="8" t="s">
-        <v>121</v>
-      </c>
       <c r="H11" s="8" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="I11" s="8">
         <v>1</v>
@@ -5760,18 +5739,18 @@
         <v>22391.718679361577</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C12" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E12" s="8" t="s">
         <v>77</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>80</v>
       </c>
       <c r="F12" s="8">
         <v>2021</v>
@@ -5791,50 +5770,50 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7:H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" style="8"/>
-    <col min="2" max="2" width="30.7265625" style="8" customWidth="1"/>
-    <col min="3" max="3" width="13.54296875" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.1796875" style="8"/>
-    <col min="5" max="5" width="16.453125" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7265625" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.26953125" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.1796875" style="8"/>
-    <col min="9" max="9" width="13.1796875" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.1796875" style="8" customWidth="1"/>
-    <col min="11" max="11" width="8.453125" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="36.54296875" style="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.1796875" style="8"/>
+    <col min="1" max="1" width="9.140625" style="8"/>
+    <col min="2" max="2" width="30.7109375" style="8" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="8"/>
+    <col min="5" max="5" width="18.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="8"/>
+    <col min="9" max="9" width="13.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" style="8" customWidth="1"/>
+    <col min="11" max="11" width="12" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="36.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="str">
         <f>"~UC_Sets: R_S: " &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!D3:AD3)</f>
         <v>~UC_Sets: R_S: National,IE-CW,IE-D,IE-KE,IE-KK,IE-LS,IE-LD,IE-LH,IE-MH,IE-OY,IE-WH,IE-WX,IE-WW,IE-CE,IE-CO,IE-KY,IE-LK,IE-TA,IE-WD,IE-G,IE-LM,IE-MO,IE-RN,IE-SO,IE-CN,IE-DL,IE-MN</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B3" s="11" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H4" s="8" t="str">
         <f>IF(RIGHT(B2,1)&lt;&gt;" ","~UC_T","")</f>
         <v>~UC_T</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B5" s="12" t="s">
         <v>61</v>
       </c>
@@ -5842,25 +5821,25 @@
         <v>62</v>
       </c>
       <c r="D5" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="F5" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="E5" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="F5" s="13" t="s">
-        <v>72</v>
-      </c>
       <c r="G5" s="13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H5" s="13" t="s">
         <v>0</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>74</v>
+        <v>118</v>
       </c>
       <c r="J5" s="14" t="s">
-        <v>78</v>
+        <v>119</v>
       </c>
       <c r="K5" s="10" t="s">
         <v>67</v>
@@ -5869,9 +5848,9 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B6" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
@@ -5882,31 +5861,28 @@
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
       <c r="K6" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L6" s="9"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F7" s="8">
         <v>2021</v>
       </c>
-      <c r="G7" s="8" t="s">
-        <v>121</v>
-      </c>
       <c r="H7" s="8" t="s">
-        <v>68</v>
+        <v>120</v>
       </c>
       <c r="I7" s="8">
         <v>1</v>
@@ -5915,27 +5891,24 @@
         <v>10174</v>
       </c>
       <c r="L7" s="8" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C8" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="F8" s="8">
         <v>2021</v>
       </c>
-      <c r="G8" s="8" t="s">
-        <v>121</v>
-      </c>
       <c r="H8" s="8" t="s">
-        <v>68</v>
+        <v>120</v>
       </c>
       <c r="I8" s="8">
         <v>1</v>
@@ -5944,27 +5917,24 @@
         <v>8680.32</v>
       </c>
       <c r="L8" s="8" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C9" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F9" s="8">
         <v>2021</v>
       </c>
-      <c r="G9" s="8" t="s">
-        <v>121</v>
-      </c>
       <c r="H9" s="8" t="s">
-        <v>68</v>
+        <v>120</v>
       </c>
       <c r="I9" s="8">
         <v>1</v>
@@ -5973,27 +5943,24 @@
         <v>10088</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C10" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F10" s="8">
         <v>2021</v>
       </c>
-      <c r="G10" s="8" t="s">
-        <v>121</v>
-      </c>
       <c r="H10" s="8" t="s">
-        <v>68</v>
+        <v>120</v>
       </c>
       <c r="I10" s="8">
         <v>1</v>
@@ -6002,27 +5969,24 @@
         <v>9817.9359360518702</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C11" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F11" s="8">
         <v>2021</v>
       </c>
-      <c r="G11" s="8" t="s">
-        <v>121</v>
-      </c>
       <c r="H11" s="8" t="s">
-        <v>68</v>
+        <v>120</v>
       </c>
       <c r="I11" s="8">
         <v>1</v>
@@ -6031,18 +5995,18 @@
         <v>22391.718679361577</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C12" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="E12" s="8" t="s">
         <v>77</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>80</v>
       </c>
       <c r="F12" s="8">
         <v>2021</v>

</xml_diff>

<commit_message>
Update 2021 sectoral carbon emissions
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_SectoralEmissions_2021.xlsx
+++ b/SuppXLS/Scen_SectoralEmissions_2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agaur\Documents\Veda\times-ireland-model-sectoral_cb\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C21B850-4AC6-47D7-B69F-B0F36C32DAD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E210688A-C0E9-40DA-A1F6-DC14A894ECEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="12600" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="17640" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="24" r:id="rId1"/>
@@ -160,7 +160,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="131">
   <si>
     <t>LimType</t>
   </si>
@@ -494,18 +494,9 @@
     <t>CO2 (Mt) in 2021</t>
   </si>
   <si>
-    <t>UC_CO2_2021_Single</t>
-  </si>
-  <si>
-    <t>SRVCO2N, RSDCO2</t>
-  </si>
-  <si>
     <t>INDCO2N,INDCO2P</t>
   </si>
   <si>
-    <t>UC_CO2_2021_Multi</t>
-  </si>
-  <si>
     <t>CO2 emissions 2021 in Transport- single</t>
   </si>
   <si>
@@ -524,9 +515,6 @@
     <t>CO2 emissions 2021 in Transport- multi</t>
   </si>
   <si>
-    <t>CO2 emissions 2021 in Buildings- multi</t>
-  </si>
-  <si>
     <t>CO2 emissions 2021 in Power- multi</t>
   </si>
   <si>
@@ -542,7 +530,49 @@
     <t>UC_FLO</t>
   </si>
   <si>
-    <t>FX</t>
+    <t>UC_CO2_2021_TRA_Single</t>
+  </si>
+  <si>
+    <t>UC_CO2_2021_RSD_Single</t>
+  </si>
+  <si>
+    <t>UC_CO2_2021_SRV_Single</t>
+  </si>
+  <si>
+    <t>UC_CO2_2021_PWR_Single</t>
+  </si>
+  <si>
+    <t>UC_CO2_2021_IND_Single</t>
+  </si>
+  <si>
+    <t>UC_CO2_2021_AGR_Single</t>
+  </si>
+  <si>
+    <t>UP</t>
+  </si>
+  <si>
+    <t>CO2 emissions 2021 in RSD- multi</t>
+  </si>
+  <si>
+    <t>CO2 emissions 2021 in SRV- multi</t>
+  </si>
+  <si>
+    <t>UC_CO2_2021_TRA_Multi</t>
+  </si>
+  <si>
+    <t>UC_CO2_2021_RSD_Multi</t>
+  </si>
+  <si>
+    <t>UC_CO2_2021_SRV_Multi</t>
+  </si>
+  <si>
+    <t>UC_CO2_2021_PWR_Multi</t>
+  </si>
+  <si>
+    <t>UC_CO2_2021_IND_Multi</t>
+  </si>
+  <si>
+    <t>UC_CO2_2021_AGR_Multi</t>
   </si>
 </sst>
 </file>
@@ -5506,52 +5536,51 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9318C9B-7F0A-410C-BCB5-F22D93E1F454}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="8"/>
     <col min="2" max="2" width="31" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" style="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.140625" style="8"/>
     <col min="5" max="5" width="16.42578125" style="8" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.7109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="8"/>
-    <col min="9" max="9" width="13.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" style="8" customWidth="1"/>
-    <col min="11" max="11" width="12" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="27.85546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="8"/>
+    <col min="7" max="7" width="9.140625" style="8"/>
+    <col min="8" max="8" width="13.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.140625" style="8" customWidth="1"/>
+    <col min="10" max="10" width="12" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="36.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="str">
         <f>"~UC_Sets: R_E: "  &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!C3)</f>
         <v>~UC_Sets: R_E: IE</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3" s="11" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H4" s="8" t="str">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G4" s="8" t="str">
         <f>IF(RIGHT(B2,1)&lt;&gt;" ","~UC_T","")</f>
         <v>~UC_T</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" s="12" t="s">
         <v>61</v>
       </c>
@@ -5568,25 +5597,22 @@
         <v>71</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="H5" s="13" t="s">
         <v>0</v>
       </c>
+      <c r="H5" s="14" t="s">
+        <v>114</v>
+      </c>
       <c r="I5" s="14" t="s">
-        <v>118</v>
-      </c>
-      <c r="J5" s="14" t="s">
-        <v>119</v>
-      </c>
-      <c r="K5" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="J5" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="L5" s="12" t="s">
+      <c r="K5" s="12" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B6" s="9" t="s">
         <v>68</v>
       </c>
@@ -5597,44 +5623,40 @@
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9" t="s">
+      <c r="J6" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="L6" s="15"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K6" s="15"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>75</v>
+        <v>116</v>
+      </c>
+      <c r="C7" s="8" t="str">
+        <f>config!C2</f>
+        <v>TRACO2N</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="E7" s="8" t="str">
-        <f>config!C2</f>
-        <v>TRACO2N</v>
-      </c>
       <c r="F7" s="8">
         <v>2021</v>
       </c>
-      <c r="H7" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="I7" s="8">
+      <c r="G7" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="H7" s="8">
         <v>1</v>
       </c>
-      <c r="K7" s="8">
+      <c r="J7" s="8">
         <f>config!D2*1000</f>
         <v>10174</v>
       </c>
-      <c r="L7" s="8" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K7" s="8" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C8" s="8" t="s">
         <v>75</v>
       </c>
@@ -5642,121 +5664,145 @@
         <v>74</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>105</v>
+        <v>77</v>
       </c>
       <c r="F8" s="8">
         <v>2021</v>
       </c>
-      <c r="H8" s="8" t="s">
-        <v>120</v>
-      </c>
       <c r="I8" s="8">
-        <v>1</v>
-      </c>
-      <c r="K8" s="8">
-        <f>config!D3*1000</f>
-        <v>8680.32</v>
-      </c>
-      <c r="L8" s="8" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B9" s="8" t="s">
+        <v>117</v>
+      </c>
       <c r="C9" s="8" t="s">
-        <v>75</v>
+        <v>98</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="E9" s="8" t="s">
-        <v>78</v>
-      </c>
       <c r="F9" s="8">
         <v>2021</v>
       </c>
-      <c r="H9" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="I9" s="8">
+      <c r="G9" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="H9" s="8">
         <v>1</v>
       </c>
-      <c r="K9" s="8">
+      <c r="J9" s="8">
+        <f>0.8*config!D3*1000</f>
+        <v>6944.2560000000003</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B10" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F10" s="8">
+        <v>2021</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="H10" s="8">
+        <v>1</v>
+      </c>
+      <c r="J10" s="8">
+        <f>0.2*config!D3</f>
+        <v>1.7360640000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B11" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F11" s="8">
+        <v>2021</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="H11" s="8">
+        <v>1</v>
+      </c>
+      <c r="J11" s="8">
         <f>config!D5*1000</f>
         <v>10088</v>
       </c>
-      <c r="L9" s="8" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C10" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="D10" s="8" t="s">
+      <c r="K11" s="8" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="D12" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="E10" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="F10" s="8">
+      <c r="F12" s="8">
         <v>2021</v>
       </c>
-      <c r="H10" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="I10" s="8">
+      <c r="G12" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="H12" s="8">
         <v>1</v>
       </c>
-      <c r="K10" s="8">
+      <c r="J12" s="8">
         <f>config!D6*1000</f>
         <v>9817.9359360518702</v>
       </c>
-      <c r="L10" s="8" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C11" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="D11" s="8" t="s">
+      <c r="K12" s="8" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D13" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="E11" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="F11" s="8">
+      <c r="F13" s="8">
         <v>2021</v>
       </c>
-      <c r="H11" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="I11" s="8">
+      <c r="G13" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="H13" s="8">
         <v>1</v>
       </c>
-      <c r="K11" s="8">
+      <c r="J13" s="8">
         <f>config!D8*1000</f>
         <v>22391.718679361577</v>
       </c>
-      <c r="L11" s="8" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C12" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="F12" s="8">
-        <v>2021</v>
-      </c>
-      <c r="J12" s="8">
-        <v>-1</v>
+      <c r="K13" s="8" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -5768,10 +5814,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6EC2971-91FC-4261-B0BB-58C7F43C1746}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7:H11"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5836,10 +5882,10 @@
         <v>0</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="J5" s="14" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="K5" s="10" t="s">
         <v>67</v>
@@ -5867,31 +5913,28 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
-        <v>107</v>
+        <v>125</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="E7" s="8" t="s">
-        <v>96</v>
-      </c>
       <c r="F7" s="8">
         <v>2021</v>
       </c>
-      <c r="H7" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="I7" s="8">
+      <c r="G7" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="H7" s="8">
         <v>1</v>
       </c>
       <c r="K7" s="8">
         <v>10174</v>
       </c>
       <c r="L7" s="8" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -5902,117 +5945,148 @@
         <v>74</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>105</v>
+        <v>77</v>
       </c>
       <c r="F8" s="8">
         <v>2021</v>
       </c>
-      <c r="H8" s="8" t="s">
-        <v>120</v>
-      </c>
       <c r="I8" s="8">
-        <v>1</v>
-      </c>
-      <c r="K8" s="8">
-        <v>8680.32</v>
-      </c>
-      <c r="L8" s="8" t="s">
-        <v>114</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B9" s="8" t="s">
+        <v>126</v>
+      </c>
       <c r="C9" s="8" t="s">
-        <v>75</v>
+        <v>98</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="E9" s="8" t="s">
-        <v>78</v>
-      </c>
       <c r="F9" s="8">
         <v>2021</v>
       </c>
-      <c r="H9" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="I9" s="8">
+      <c r="G9" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="H9" s="8">
         <v>1</v>
       </c>
       <c r="K9" s="8">
-        <v>10088</v>
+        <f>0.8*8680.32</f>
+        <v>6944.2560000000003</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B10" s="8" t="s">
+        <v>127</v>
+      </c>
       <c r="C10" s="8" t="s">
-        <v>75</v>
+        <v>97</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="E10" s="8" t="s">
-        <v>106</v>
-      </c>
       <c r="F10" s="8">
         <v>2021</v>
       </c>
-      <c r="H10" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="I10" s="8">
+      <c r="G10" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="H10" s="8">
         <v>1</v>
       </c>
       <c r="K10" s="8">
-        <v>9817.9359360518702</v>
+        <f>single!J10</f>
+        <v>1.7360640000000001</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B11" s="8" t="s">
+        <v>128</v>
+      </c>
       <c r="C11" s="8" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="D11" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="E11" s="8" t="s">
-        <v>101</v>
-      </c>
       <c r="F11" s="8">
         <v>2021</v>
       </c>
-      <c r="H11" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="I11" s="8">
+      <c r="G11" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="H11" s="8">
         <v>1</v>
       </c>
       <c r="K11" s="8">
-        <v>22391.718679361577</v>
+        <v>10088</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B12" s="8" t="s">
+        <v>129</v>
+      </c>
       <c r="C12" s="8" t="s">
-        <v>75</v>
+        <v>104</v>
       </c>
       <c r="D12" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="E12" s="8" t="s">
-        <v>77</v>
-      </c>
       <c r="F12" s="8">
         <v>2021</v>
       </c>
+      <c r="G12" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="H12" s="8">
+        <v>1</v>
+      </c>
       <c r="J12" s="8">
         <v>-1</v>
+      </c>
+      <c r="K12" s="8">
+        <v>9817.9359360518702</v>
+      </c>
+      <c r="L12" s="8" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B13" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="F13" s="8">
+        <v>2021</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="H13" s="8">
+        <v>1</v>
+      </c>
+      <c r="K13" s="8">
+        <v>22391.718679361577</v>
+      </c>
+      <c r="L13" s="8" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>